<commit_message>
Removed previous physical and financial programs when duplicating rows
</commit_message>
<xml_diff>
--- a/public/BLD-BE-001 Budget Estimate template.xlsx
+++ b/public/BLD-BE-001 Budget Estimate template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27123"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27226"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - Department of Education\tld\Caracas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E4FB1D2D-4C0E-4292-8F6C-1758629ECE9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{13E0EA9C-071B-44AA-A200-B18A4CA1B048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11736" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="115">
   <si>
     <t>BLD-BE-001</t>
   </si>
@@ -132,243 +132,246 @@
     <t>VENUE:</t>
   </si>
   <si>
+    <t>TANZA, CAVITE</t>
+  </si>
+  <si>
+    <t>ITEMS</t>
+  </si>
+  <si>
+    <t>No. of Pax</t>
+  </si>
+  <si>
+    <t>Days</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Direct Payment</t>
+  </si>
+  <si>
+    <t>Cash Advance</t>
+  </si>
+  <si>
+    <t>Downloading</t>
+  </si>
+  <si>
+    <t>Board and Lodging</t>
+  </si>
+  <si>
+    <t>Participants</t>
+  </si>
+  <si>
+    <t>Resource Persons</t>
+  </si>
+  <si>
+    <t>Technical Experts ( Editors/Validators/Illustrators)</t>
+  </si>
+  <si>
+    <t>Bureau of Learning Delivery</t>
+  </si>
+  <si>
+    <t>Office of the Director</t>
+  </si>
+  <si>
+    <t>TLD</t>
+  </si>
+  <si>
+    <t>SID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other Offices </t>
+  </si>
+  <si>
+    <t>Curriculum &amp; Teaching</t>
+  </si>
+  <si>
+    <t>Other Invited Offices</t>
+  </si>
+  <si>
+    <t>Travel Expenses</t>
+  </si>
+  <si>
+    <t>Region I</t>
+  </si>
+  <si>
+    <t>Region II</t>
+  </si>
+  <si>
+    <t>Batanes</t>
+  </si>
+  <si>
+    <t>Region III</t>
+  </si>
+  <si>
+    <t>Calabarzon</t>
+  </si>
+  <si>
+    <t>Mimaropa</t>
+  </si>
+  <si>
+    <t>Palawan</t>
+  </si>
+  <si>
+    <t>Region V</t>
+  </si>
+  <si>
+    <t>CAR</t>
+  </si>
+  <si>
+    <t>NCR</t>
+  </si>
+  <si>
+    <t>Region VI</t>
+  </si>
+  <si>
+    <t>Region VII</t>
+  </si>
+  <si>
+    <t>Region VIII</t>
+  </si>
+  <si>
+    <t>Region IX</t>
+  </si>
+  <si>
+    <t>Region X</t>
+  </si>
+  <si>
+    <t>Region XI</t>
+  </si>
+  <si>
+    <t>Region XII</t>
+  </si>
+  <si>
+    <t>CARAGA</t>
+  </si>
+  <si>
+    <t>BARMM</t>
+  </si>
+  <si>
+    <t>Honorarium of Non Deped Personnel</t>
+  </si>
+  <si>
+    <t>Meal Expenses</t>
+  </si>
+  <si>
+    <t>Supplies and Materials</t>
+  </si>
+  <si>
+    <t>Contingency</t>
+  </si>
+  <si>
+    <t>Sub-Total</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Prepared:</t>
+  </si>
+  <si>
+    <t>Reviewed:</t>
+  </si>
+  <si>
+    <t>Recommending Approval:</t>
+  </si>
+  <si>
+    <t>Approved:</t>
+  </si>
+  <si>
+    <t>Focal Person - SEPS</t>
+  </si>
+  <si>
+    <t>SVEPS</t>
+  </si>
+  <si>
+    <t>CHIEF</t>
+  </si>
+  <si>
+    <t>DIRECTOR</t>
+  </si>
+  <si>
+    <t>Pax Greater Than</t>
+  </si>
+  <si>
+    <t>Pax Less Than Equal to</t>
+  </si>
+  <si>
+    <t>Transportation Expenses per Venue ( as of April 29, 2019)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Venues </t>
+  </si>
+  <si>
+    <t>CLUSTER DTE</t>
+  </si>
+  <si>
+    <t>Without  Changes</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>BATANES</t>
+  </si>
+  <si>
+    <t>PALAWAN</t>
+  </si>
+  <si>
+    <t>BACOLOD</t>
+  </si>
+  <si>
+    <t>BAGUIO CITY</t>
+  </si>
+  <si>
+    <t>BATAAN</t>
+  </si>
+  <si>
+    <t>BATANGAS MALVAR</t>
+  </si>
+  <si>
+    <t>BORACAY</t>
+  </si>
+  <si>
+    <t>BUTUAN</t>
+  </si>
+  <si>
+    <t>CABANATUAN</t>
+  </si>
+  <si>
+    <t>CAG. DE ORO</t>
+  </si>
+  <si>
+    <t>CEBU CITY</t>
+  </si>
+  <si>
+    <t>DAVAO CITY</t>
+  </si>
+  <si>
+    <t>DUMAGUETE</t>
+  </si>
+  <si>
+    <t>GENERAL SANTOS</t>
+  </si>
+  <si>
+    <t>ILOILO CITY</t>
+  </si>
+  <si>
+    <t>KORONADAL</t>
+  </si>
+  <si>
+    <t>LA UNION</t>
+  </si>
+  <si>
+    <t>LEGASPI</t>
+  </si>
+  <si>
     <t>LOS BANOS</t>
   </si>
   <si>
-    <t>ITEMS</t>
-  </si>
-  <si>
-    <t>No. of Pax</t>
-  </si>
-  <si>
-    <t>Days</t>
-  </si>
-  <si>
-    <t>Amount</t>
-  </si>
-  <si>
-    <t>TOTAL</t>
-  </si>
-  <si>
-    <t>Direct Payment</t>
-  </si>
-  <si>
-    <t>Cash Advance</t>
-  </si>
-  <si>
-    <t>Downloading</t>
-  </si>
-  <si>
-    <t>Board and Lodging</t>
-  </si>
-  <si>
-    <t>Participants</t>
-  </si>
-  <si>
-    <t>Resource Persons</t>
-  </si>
-  <si>
-    <t>Technical Experts ( Editors/Validators/Illustrators)</t>
-  </si>
-  <si>
-    <t>Bureau of Learning Delivery</t>
-  </si>
-  <si>
-    <t>Office of the Director</t>
-  </si>
-  <si>
-    <t>TLD</t>
-  </si>
-  <si>
-    <t>SID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other Offices </t>
-  </si>
-  <si>
-    <t>Curriculum &amp; Teaching</t>
-  </si>
-  <si>
-    <t>Other Invited Offices</t>
-  </si>
-  <si>
-    <t>Travel Expenses</t>
-  </si>
-  <si>
-    <t>Region I</t>
-  </si>
-  <si>
-    <t>Region II</t>
-  </si>
-  <si>
-    <t>Batanes</t>
-  </si>
-  <si>
-    <t>Region III</t>
-  </si>
-  <si>
-    <t>Calabarzon</t>
-  </si>
-  <si>
-    <t>Mimaropa</t>
-  </si>
-  <si>
-    <t>Palawan</t>
-  </si>
-  <si>
-    <t>Region V</t>
-  </si>
-  <si>
-    <t>CAR</t>
-  </si>
-  <si>
-    <t>NCR</t>
-  </si>
-  <si>
-    <t>Region VI</t>
-  </si>
-  <si>
-    <t>Region VII</t>
-  </si>
-  <si>
-    <t>Region VIII</t>
-  </si>
-  <si>
-    <t>Region IX</t>
-  </si>
-  <si>
-    <t>Region X</t>
-  </si>
-  <si>
-    <t>Region XI</t>
-  </si>
-  <si>
-    <t>Region XII</t>
-  </si>
-  <si>
-    <t>CARAGA</t>
-  </si>
-  <si>
-    <t>BARMM</t>
-  </si>
-  <si>
-    <t>Honorarium of Non Deped Personnel</t>
-  </si>
-  <si>
-    <t>Meal Expenses</t>
-  </si>
-  <si>
-    <t>Supplies and Materials</t>
-  </si>
-  <si>
-    <t>Contingency</t>
-  </si>
-  <si>
-    <t>Sub-Total</t>
-  </si>
-  <si>
-    <t>Grand Total</t>
-  </si>
-  <si>
-    <t>Prepared:</t>
-  </si>
-  <si>
-    <t>Reviewed:</t>
-  </si>
-  <si>
-    <t>Recommending Approval:</t>
-  </si>
-  <si>
-    <t>Approved:</t>
-  </si>
-  <si>
-    <t>Focal Person - SEPS</t>
-  </si>
-  <si>
-    <t>SVEPS</t>
-  </si>
-  <si>
-    <t>CHIEF</t>
-  </si>
-  <si>
-    <t>DIRECTOR</t>
-  </si>
-  <si>
-    <t>Pax Greater Than</t>
-  </si>
-  <si>
-    <t>Pax Less Than Equal to</t>
-  </si>
-  <si>
-    <t>Transportation Expenses per Venue ( as of April 29, 2019)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Venues </t>
-  </si>
-  <si>
-    <t>CLUSTER DTE</t>
-  </si>
-  <si>
-    <t>Without  Changes</t>
-  </si>
-  <si>
-    <t>CO</t>
-  </si>
-  <si>
-    <t>BATANES</t>
-  </si>
-  <si>
-    <t>PALAWAN</t>
-  </si>
-  <si>
-    <t>BACOLOD</t>
-  </si>
-  <si>
-    <t>BAGUIO CITY</t>
-  </si>
-  <si>
-    <t>BATAAN</t>
-  </si>
-  <si>
-    <t>BATANGAS MALVAR</t>
-  </si>
-  <si>
-    <t>BORACAY</t>
-  </si>
-  <si>
-    <t>BUTUAN</t>
-  </si>
-  <si>
-    <t>CABANATUAN</t>
-  </si>
-  <si>
-    <t>CAG. DE ORO</t>
-  </si>
-  <si>
-    <t>CEBU CITY</t>
-  </si>
-  <si>
-    <t>DAVAO CITY</t>
-  </si>
-  <si>
-    <t>DUMAGUETE</t>
-  </si>
-  <si>
-    <t>GENERAL SANTOS</t>
-  </si>
-  <si>
-    <t>ILOILO CITY</t>
-  </si>
-  <si>
-    <t>KORONADAL</t>
-  </si>
-  <si>
-    <t>LA UNION</t>
-  </si>
-  <si>
-    <t>LEGASPI</t>
-  </si>
-  <si>
     <t>MARIKINA</t>
   </si>
   <si>
@@ -406,9 +409,6 @@
   </si>
   <si>
     <t>TANAY / ANTIPOLO</t>
-  </si>
-  <si>
-    <t>TANZA, CAVITE</t>
   </si>
   <si>
     <t>TUGUEGARAO</t>
@@ -425,8 +425,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@"/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -1375,7 +1375,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="223">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1528,28 +1528,28 @@
     <xf numFmtId="0" fontId="22" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="16" fillId="24" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="21" fillId="24" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="25" fillId="24" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="14" fillId="24" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="16" fillId="24" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="21" fillId="24" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="25" fillId="24" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="14" fillId="24" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="24" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="16" fillId="24" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="22" fillId="24" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="16" fillId="24" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="16" fillId="24" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="22" fillId="24" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="16" fillId="24" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="25" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="25" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="18" fillId="25" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="18" fillId="25" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="18" fillId="25" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="15" fillId="26" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="18" fillId="26" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="15" fillId="29" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="15" fillId="30" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="16" fillId="31" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="18" fillId="25" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="18" fillId="25" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="18" fillId="25" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="15" fillId="26" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="18" fillId="26" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="15" fillId="29" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="15" fillId="30" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="16" fillId="31" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="31" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="18" fillId="31" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="18" fillId="31" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="31" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="18" fillId="31" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="18" fillId="31" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1568,224 +1568,224 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="22" fillId="22" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="20" fillId="23" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="22" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="20" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="22" fillId="22" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="20" fillId="23" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="14" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="17" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="22" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="22" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="22" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="14" fillId="20" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="14" fillId="20" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="14" fillId="22" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="17" fillId="23" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="43" fontId="20" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="22" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="22" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="14" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="20" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="22" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="23" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="20" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="20" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="22" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="23" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="22" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="23" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="22" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="20" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -2074,8 +2074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A34" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="J60" sqref="J60"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2100,7 +2100,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" thickBot="1">
-      <c r="A1" s="114"/>
+      <c r="A1" s="182"/>
       <c r="B1" s="187"/>
       <c r="C1" s="187"/>
       <c r="D1" s="187"/>
@@ -2142,12 +2142,12 @@
     <row r="3" spans="1:17" ht="14.45">
       <c r="A3" s="51"/>
       <c r="B3" s="52"/>
-      <c r="C3" s="115" t="s">
+      <c r="C3" s="165" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="189"/>
       <c r="E3" s="190"/>
-      <c r="F3" s="116" t="s">
+      <c r="F3" s="183" t="s">
         <v>2</v>
       </c>
       <c r="G3" s="191"/>
@@ -2159,18 +2159,18 @@
       <c r="M3" s="191"/>
       <c r="N3" s="191"/>
       <c r="O3" s="192"/>
-      <c r="P3" s="126"/>
+      <c r="P3" s="171"/>
       <c r="Q3" s="43"/>
     </row>
     <row r="4" spans="1:17" ht="14.45">
       <c r="A4" s="51"/>
       <c r="B4" s="52"/>
-      <c r="C4" s="115" t="s">
+      <c r="C4" s="165" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="189"/>
       <c r="E4" s="190"/>
-      <c r="F4" s="117"/>
+      <c r="F4" s="172"/>
       <c r="G4" s="193"/>
       <c r="H4" s="193"/>
       <c r="I4" s="193"/>
@@ -2180,18 +2180,18 @@
       <c r="M4" s="193"/>
       <c r="N4" s="193"/>
       <c r="O4" s="194"/>
-      <c r="P4" s="126"/>
+      <c r="P4" s="171"/>
       <c r="Q4" s="43"/>
     </row>
     <row r="5" spans="1:17">
       <c r="A5" s="51"/>
       <c r="B5" s="52"/>
-      <c r="C5" s="115" t="s">
+      <c r="C5" s="165" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="189"/>
       <c r="E5" s="190"/>
-      <c r="F5" s="118"/>
+      <c r="F5" s="184"/>
       <c r="G5" s="193"/>
       <c r="H5" s="193"/>
       <c r="I5" s="193"/>
@@ -2201,13 +2201,13 @@
       <c r="M5" s="193"/>
       <c r="N5" s="193"/>
       <c r="O5" s="194"/>
-      <c r="P5" s="126"/>
+      <c r="P5" s="171"/>
       <c r="Q5" s="43"/>
     </row>
     <row r="6" spans="1:17" ht="14.45" customHeight="1">
       <c r="A6" s="51"/>
       <c r="B6" s="52"/>
-      <c r="C6" s="119" t="s">
+      <c r="C6" s="175" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="195"/>
@@ -2218,24 +2218,24 @@
       <c r="I6" s="111"/>
       <c r="J6" s="111"/>
       <c r="K6" s="111"/>
-      <c r="L6" s="132" t="s">
+      <c r="L6" s="179" t="s">
         <v>6</v>
       </c>
-      <c r="M6" s="133"/>
-      <c r="N6" s="134"/>
+      <c r="M6" s="180"/>
+      <c r="N6" s="181"/>
       <c r="O6" s="112"/>
-      <c r="P6" s="126"/>
+      <c r="P6" s="171"/>
       <c r="Q6" s="43"/>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="51"/>
       <c r="B7" s="52"/>
-      <c r="C7" s="115" t="s">
+      <c r="C7" s="165" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="189"/>
       <c r="E7" s="190"/>
-      <c r="F7" s="118"/>
+      <c r="F7" s="184"/>
       <c r="G7" s="193"/>
       <c r="H7" s="193"/>
       <c r="I7" s="193"/>
@@ -2245,13 +2245,13 @@
       <c r="M7" s="193"/>
       <c r="N7" s="193"/>
       <c r="O7" s="194"/>
-      <c r="P7" s="126"/>
+      <c r="P7" s="171"/>
       <c r="Q7" s="43"/>
     </row>
     <row r="8" spans="1:17" ht="14.45" customHeight="1">
       <c r="A8" s="51"/>
       <c r="B8" s="52"/>
-      <c r="C8" s="119" t="s">
+      <c r="C8" s="175" t="s">
         <v>8</v>
       </c>
       <c r="D8" s="195"/>
@@ -2262,66 +2262,66 @@
       <c r="I8" s="111"/>
       <c r="J8" s="111"/>
       <c r="K8" s="111"/>
-      <c r="L8" s="132" t="s">
+      <c r="L8" s="179" t="s">
         <v>9</v>
       </c>
-      <c r="M8" s="133"/>
-      <c r="N8" s="134"/>
+      <c r="M8" s="180"/>
+      <c r="N8" s="181"/>
       <c r="O8" s="112"/>
-      <c r="P8" s="126"/>
+      <c r="P8" s="171"/>
       <c r="Q8" s="43"/>
     </row>
     <row r="9" spans="1:17">
       <c r="A9" s="51"/>
       <c r="B9" s="52"/>
-      <c r="C9" s="129" t="s">
+      <c r="C9" s="176" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="130"/>
-      <c r="E9" s="131"/>
-      <c r="F9" s="117"/>
-      <c r="G9" s="127"/>
-      <c r="H9" s="127"/>
-      <c r="I9" s="127"/>
-      <c r="J9" s="127"/>
-      <c r="K9" s="127"/>
-      <c r="L9" s="127"/>
-      <c r="M9" s="127"/>
-      <c r="N9" s="127"/>
-      <c r="O9" s="128"/>
-      <c r="P9" s="126"/>
+      <c r="D9" s="177"/>
+      <c r="E9" s="178"/>
+      <c r="F9" s="172"/>
+      <c r="G9" s="173"/>
+      <c r="H9" s="173"/>
+      <c r="I9" s="173"/>
+      <c r="J9" s="173"/>
+      <c r="K9" s="173"/>
+      <c r="L9" s="173"/>
+      <c r="M9" s="173"/>
+      <c r="N9" s="173"/>
+      <c r="O9" s="174"/>
+      <c r="P9" s="171"/>
       <c r="Q9" s="43"/>
     </row>
     <row r="10" spans="1:17" ht="14.45">
       <c r="A10" s="51"/>
       <c r="B10" s="52"/>
-      <c r="C10" s="119" t="s">
+      <c r="C10" s="175" t="s">
         <v>11</v>
       </c>
       <c r="D10" s="195"/>
       <c r="E10" s="196"/>
-      <c r="F10" s="117"/>
-      <c r="G10" s="127"/>
-      <c r="H10" s="127"/>
-      <c r="I10" s="127"/>
-      <c r="J10" s="127"/>
-      <c r="K10" s="127"/>
-      <c r="L10" s="127"/>
-      <c r="M10" s="127"/>
-      <c r="N10" s="127"/>
-      <c r="O10" s="128"/>
-      <c r="P10" s="126"/>
+      <c r="F10" s="172"/>
+      <c r="G10" s="173"/>
+      <c r="H10" s="173"/>
+      <c r="I10" s="173"/>
+      <c r="J10" s="173"/>
+      <c r="K10" s="173"/>
+      <c r="L10" s="173"/>
+      <c r="M10" s="173"/>
+      <c r="N10" s="173"/>
+      <c r="O10" s="174"/>
+      <c r="P10" s="171"/>
       <c r="Q10" s="43"/>
     </row>
     <row r="11" spans="1:17" ht="14.45">
       <c r="A11" s="51"/>
       <c r="B11" s="52"/>
-      <c r="C11" s="115" t="s">
+      <c r="C11" s="165" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="189"/>
       <c r="E11" s="190"/>
-      <c r="F11" s="120"/>
+      <c r="F11" s="166"/>
       <c r="G11" s="193"/>
       <c r="H11" s="193"/>
       <c r="I11" s="193"/>
@@ -2331,7 +2331,7 @@
       <c r="M11" s="193"/>
       <c r="N11" s="193"/>
       <c r="O11" s="194"/>
-      <c r="P11" s="126"/>
+      <c r="P11" s="171"/>
       <c r="Q11" s="104"/>
     </row>
     <row r="12" spans="1:17" thickBot="1">
@@ -2360,7 +2360,7 @@
     <row r="13" spans="1:17" ht="14.45">
       <c r="A13" s="51"/>
       <c r="B13" s="52"/>
-      <c r="C13" s="121" t="s">
+      <c r="C13" s="167" t="s">
         <v>14</v>
       </c>
       <c r="D13" s="197"/>
@@ -2369,16 +2369,16 @@
         <v>15</v>
       </c>
       <c r="G13" s="54">
-        <v>45241</v>
-      </c>
-      <c r="H13" s="122" t="s">
+        <v>45334</v>
+      </c>
+      <c r="H13" s="168" t="s">
         <v>16</v>
       </c>
       <c r="I13" s="198"/>
       <c r="J13" s="54">
-        <v>45243</v>
-      </c>
-      <c r="K13" s="122" t="s">
+        <v>45336</v>
+      </c>
+      <c r="K13" s="168" t="s">
         <v>17</v>
       </c>
       <c r="L13" s="198"/>
@@ -2389,10 +2389,12 @@
       <c r="N13" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="O13" s="123" t="s">
+      <c r="O13" s="169" t="s">
         <v>19</v>
       </c>
-      <c r="P13" s="199"/>
+      <c r="P13" s="199" t="s">
+        <v>19</v>
+      </c>
       <c r="Q13" s="3"/>
     </row>
     <row r="14" spans="1:17" ht="7.5" customHeight="1" thickBot="1">
@@ -2415,7 +2417,7 @@
       <c r="Q14" s="4"/>
     </row>
     <row r="15" spans="1:17" ht="24">
-      <c r="A15" s="124" t="s">
+      <c r="A15" s="170" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="200"/>
@@ -2424,14 +2426,14 @@
       <c r="E15" s="200"/>
       <c r="F15" s="200"/>
       <c r="G15" s="201"/>
-      <c r="H15" s="125" t="s">
+      <c r="H15" s="162" t="s">
         <v>21</v>
       </c>
       <c r="I15" s="201"/>
       <c r="J15" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="K15" s="125" t="s">
+      <c r="K15" s="162" t="s">
         <v>23</v>
       </c>
       <c r="L15" s="201"/>
@@ -2451,7 +2453,7 @@
     </row>
     <row r="16" spans="1:17" ht="14.45">
       <c r="A16" s="62"/>
-      <c r="B16" s="143" t="s">
+      <c r="B16" s="132" t="s">
         <v>28</v>
       </c>
       <c r="C16" s="202"/>
@@ -2459,7 +2461,7 @@
       <c r="E16" s="202"/>
       <c r="F16" s="202"/>
       <c r="G16" s="203"/>
-      <c r="H16" s="144">
+      <c r="H16" s="164">
         <f>H17+H18+H19+H20+H24</f>
         <v>0</v>
       </c>
@@ -2482,14 +2484,14 @@
     <row r="17" spans="1:17" s="46" customFormat="1" ht="14.25" customHeight="1">
       <c r="A17" s="64"/>
       <c r="B17" s="68"/>
-      <c r="C17" s="145" t="s">
+      <c r="C17" s="131" t="s">
         <v>29</v>
       </c>
       <c r="D17" s="205"/>
       <c r="E17" s="205"/>
       <c r="F17" s="205"/>
       <c r="G17" s="206"/>
-      <c r="H17" s="144">
+      <c r="H17" s="164">
         <f>H28</f>
         <v>0</v>
       </c>
@@ -2498,10 +2500,10 @@
         <f>NDAYS</f>
         <v>2</v>
       </c>
-      <c r="K17" s="138">
+      <c r="K17" s="158">
         <v>2000</v>
       </c>
-      <c r="L17" s="139"/>
+      <c r="L17" s="163"/>
       <c r="M17" s="77">
         <f t="shared" ref="M17:M20" si="0">H17*J17*K17</f>
         <v>0</v>
@@ -2514,14 +2516,14 @@
     <row r="18" spans="1:17" s="46" customFormat="1" ht="13.9">
       <c r="A18" s="64"/>
       <c r="B18" s="69"/>
-      <c r="C18" s="145" t="s">
+      <c r="C18" s="131" t="s">
         <v>30</v>
       </c>
       <c r="D18" s="205"/>
       <c r="E18" s="205"/>
       <c r="F18" s="205"/>
       <c r="G18" s="206"/>
-      <c r="H18" s="144">
+      <c r="H18" s="164">
         <f>H48</f>
         <v>0</v>
       </c>
@@ -2530,10 +2532,10 @@
         <f>NDAYS</f>
         <v>2</v>
       </c>
-      <c r="K18" s="138">
+      <c r="K18" s="158">
         <v>2000</v>
       </c>
-      <c r="L18" s="140"/>
+      <c r="L18" s="159"/>
       <c r="M18" s="77">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2546,14 +2548,14 @@
     <row r="19" spans="1:17" s="46" customFormat="1" ht="13.9">
       <c r="A19" s="64"/>
       <c r="B19" s="69"/>
-      <c r="C19" s="145" t="s">
+      <c r="C19" s="131" t="s">
         <v>31</v>
       </c>
       <c r="D19" s="205"/>
       <c r="E19" s="205"/>
       <c r="F19" s="205"/>
       <c r="G19" s="206"/>
-      <c r="H19" s="146">
+      <c r="H19" s="136">
         <f>H49</f>
         <v>0</v>
       </c>
@@ -2562,10 +2564,10 @@
         <f>NDAYS</f>
         <v>2</v>
       </c>
-      <c r="K19" s="138">
+      <c r="K19" s="158">
         <v>2000</v>
       </c>
-      <c r="L19" s="140"/>
+      <c r="L19" s="159"/>
       <c r="M19" s="77">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2578,14 +2580,14 @@
     <row r="20" spans="1:17" s="46" customFormat="1" ht="13.9">
       <c r="A20" s="64"/>
       <c r="B20" s="69"/>
-      <c r="C20" s="145" t="s">
+      <c r="C20" s="131" t="s">
         <v>32</v>
       </c>
       <c r="D20" s="205"/>
       <c r="E20" s="205"/>
       <c r="F20" s="205"/>
       <c r="G20" s="206"/>
-      <c r="H20" s="146">
+      <c r="H20" s="136">
         <f>H50</f>
         <v>0</v>
       </c>
@@ -2594,10 +2596,10 @@
         <f>NDAYS</f>
         <v>2</v>
       </c>
-      <c r="K20" s="138">
+      <c r="K20" s="158">
         <v>2000</v>
       </c>
-      <c r="L20" s="140"/>
+      <c r="L20" s="159"/>
       <c r="M20" s="77">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2611,20 +2613,20 @@
       <c r="A21" s="64"/>
       <c r="B21" s="69"/>
       <c r="C21" s="70"/>
-      <c r="D21" s="147" t="s">
+      <c r="D21" s="115" t="s">
         <v>33</v>
       </c>
       <c r="E21" s="205"/>
       <c r="F21" s="205"/>
       <c r="G21" s="206"/>
-      <c r="H21" s="148">
+      <c r="H21" s="133">
         <f>H51</f>
         <v>0</v>
       </c>
       <c r="I21" s="207"/>
       <c r="J21" s="73"/>
-      <c r="K21" s="141"/>
-      <c r="L21" s="142"/>
+      <c r="K21" s="146"/>
+      <c r="L21" s="147"/>
       <c r="M21" s="78"/>
       <c r="N21" s="94"/>
       <c r="O21" s="85"/>
@@ -2638,20 +2640,20 @@
       <c r="A22" s="64"/>
       <c r="B22" s="69"/>
       <c r="C22" s="70"/>
-      <c r="D22" s="152" t="s">
+      <c r="D22" s="154" t="s">
         <v>34</v>
       </c>
-      <c r="E22" s="153"/>
-      <c r="F22" s="153"/>
-      <c r="G22" s="154"/>
-      <c r="H22" s="148">
+      <c r="E22" s="155"/>
+      <c r="F22" s="155"/>
+      <c r="G22" s="156"/>
+      <c r="H22" s="133">
         <f>H53</f>
         <v>0</v>
       </c>
       <c r="I22" s="207"/>
       <c r="J22" s="73"/>
-      <c r="K22" s="141"/>
-      <c r="L22" s="142"/>
+      <c r="K22" s="146"/>
+      <c r="L22" s="147"/>
       <c r="M22" s="78"/>
       <c r="N22" s="94"/>
       <c r="O22" s="85"/>
@@ -2662,19 +2664,19 @@
       <c r="A23" s="64"/>
       <c r="B23" s="69"/>
       <c r="C23" s="70"/>
-      <c r="D23" s="149" t="s">
+      <c r="D23" s="127" t="s">
         <v>35</v>
       </c>
       <c r="E23" s="208"/>
       <c r="F23" s="208"/>
       <c r="G23" s="209"/>
-      <c r="H23" s="148">
+      <c r="H23" s="133">
         <f t="shared" ref="H23:H26" si="2">H53</f>
         <v>0</v>
       </c>
       <c r="I23" s="207"/>
       <c r="J23" s="73"/>
-      <c r="K23" s="141"/>
+      <c r="K23" s="146"/>
       <c r="L23" s="157"/>
       <c r="M23" s="78"/>
       <c r="N23" s="94"/>
@@ -2688,14 +2690,14 @@
     <row r="24" spans="1:17" s="46" customFormat="1" ht="13.9" customHeight="1">
       <c r="A24" s="64"/>
       <c r="B24" s="69"/>
-      <c r="C24" s="145" t="s">
+      <c r="C24" s="131" t="s">
         <v>36</v>
       </c>
       <c r="D24" s="205"/>
       <c r="E24" s="205"/>
       <c r="F24" s="205"/>
       <c r="G24" s="206"/>
-      <c r="H24" s="146">
+      <c r="H24" s="136">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2704,10 +2706,10 @@
         <f>NDAYS</f>
         <v>2</v>
       </c>
-      <c r="K24" s="138">
+      <c r="K24" s="158">
         <v>2000</v>
       </c>
-      <c r="L24" s="140"/>
+      <c r="L24" s="159"/>
       <c r="M24" s="77">
         <f>H24*J24*K24</f>
         <v>0</v>
@@ -2721,20 +2723,20 @@
       <c r="A25" s="64"/>
       <c r="B25" s="69"/>
       <c r="C25" s="70"/>
-      <c r="D25" s="147" t="s">
+      <c r="D25" s="115" t="s">
         <v>37</v>
       </c>
       <c r="E25" s="205"/>
       <c r="F25" s="205"/>
       <c r="G25" s="206"/>
-      <c r="H25" s="148">
+      <c r="H25" s="133">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I25" s="207"/>
       <c r="J25" s="63"/>
-      <c r="K25" s="158"/>
-      <c r="L25" s="136"/>
+      <c r="K25" s="129"/>
+      <c r="L25" s="130"/>
       <c r="M25" s="79"/>
       <c r="N25" s="94"/>
       <c r="O25" s="85"/>
@@ -2748,20 +2750,20 @@
       <c r="A26" s="64"/>
       <c r="B26" s="69"/>
       <c r="C26" s="70"/>
-      <c r="D26" s="147" t="s">
+      <c r="D26" s="115" t="s">
         <v>38</v>
       </c>
       <c r="E26" s="205"/>
       <c r="F26" s="205"/>
       <c r="G26" s="206"/>
-      <c r="H26" s="148">
+      <c r="H26" s="133">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I26" s="207"/>
       <c r="J26" s="63"/>
-      <c r="K26" s="158"/>
-      <c r="L26" s="136"/>
+      <c r="K26" s="129"/>
+      <c r="L26" s="130"/>
       <c r="M26" s="79"/>
       <c r="N26" s="94"/>
       <c r="O26" s="85"/>
@@ -2773,7 +2775,7 @@
     </row>
     <row r="27" spans="1:17" ht="15.75" customHeight="1">
       <c r="A27" s="64"/>
-      <c r="B27" s="143" t="s">
+      <c r="B27" s="132" t="s">
         <v>39</v>
       </c>
       <c r="C27" s="202"/>
@@ -2781,11 +2783,11 @@
       <c r="E27" s="202"/>
       <c r="F27" s="202"/>
       <c r="G27" s="203"/>
-      <c r="H27" s="151"/>
+      <c r="H27" s="160"/>
       <c r="I27" s="204"/>
       <c r="J27" s="63"/>
-      <c r="K27" s="158"/>
-      <c r="L27" s="136"/>
+      <c r="K27" s="129"/>
+      <c r="L27" s="130"/>
       <c r="M27" s="80"/>
       <c r="N27" s="94"/>
       <c r="O27" s="85"/>
@@ -2798,21 +2800,21 @@
     <row r="28" spans="1:17" ht="15.75" customHeight="1">
       <c r="A28" s="64"/>
       <c r="B28" s="68"/>
-      <c r="C28" s="145" t="s">
+      <c r="C28" s="131" t="s">
         <v>29</v>
       </c>
       <c r="D28" s="205"/>
       <c r="E28" s="205"/>
       <c r="F28" s="205"/>
       <c r="G28" s="206"/>
-      <c r="H28" s="146">
+      <c r="H28" s="136">
         <f>SUM(H29:I47)</f>
         <v>0</v>
       </c>
       <c r="I28" s="204"/>
       <c r="J28" s="63"/>
-      <c r="K28" s="135"/>
-      <c r="L28" s="136"/>
+      <c r="K28" s="161"/>
+      <c r="L28" s="130"/>
       <c r="M28" s="81">
         <f>SUM(M29:M47)</f>
         <v>0</v>
@@ -2829,22 +2831,22 @@
       <c r="A29" s="64"/>
       <c r="B29" s="69"/>
       <c r="C29" s="70"/>
-      <c r="D29" s="147" t="s">
+      <c r="D29" s="115" t="s">
         <v>40</v>
       </c>
       <c r="E29" s="205"/>
       <c r="F29" s="205"/>
       <c r="G29" s="206"/>
-      <c r="H29" s="150">
+      <c r="H29" s="116">
         <v>0</v>
       </c>
       <c r="I29" s="194"/>
       <c r="J29" s="63"/>
-      <c r="K29" s="155">
+      <c r="K29" s="118">
         <f t="shared" ref="K29:K46" si="4">IF(NDAYS&gt;1,VLOOKUP(VENUE,VENUEMATRIX,MATCH(D29,REGIONS,0),)+(VLOOKUP(VENUE,VENUEMATRIX,2)*0.2)*2,VLOOKUP(VENUE,VENUEMATRIX,MATCH(D29,REGIONS,0),))</f>
         <v>5180</v>
       </c>
-      <c r="L29" s="156"/>
+      <c r="L29" s="119"/>
       <c r="M29" s="82">
         <f t="shared" ref="M29:M56" si="5">K29*H29</f>
         <v>0</v>
@@ -2858,22 +2860,22 @@
       <c r="A30" s="64"/>
       <c r="B30" s="69"/>
       <c r="C30" s="70"/>
-      <c r="D30" s="147" t="s">
+      <c r="D30" s="115" t="s">
         <v>41</v>
       </c>
       <c r="E30" s="205"/>
       <c r="F30" s="205"/>
       <c r="G30" s="206"/>
-      <c r="H30" s="150">
+      <c r="H30" s="116">
         <v>0</v>
       </c>
       <c r="I30" s="194"/>
       <c r="J30" s="63"/>
-      <c r="K30" s="155">
+      <c r="K30" s="118">
         <f t="shared" si="4"/>
         <v>8180</v>
       </c>
-      <c r="L30" s="156"/>
+      <c r="L30" s="119"/>
       <c r="M30" s="82">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -2887,22 +2889,22 @@
       <c r="A31" s="64"/>
       <c r="B31" s="69"/>
       <c r="C31" s="70"/>
-      <c r="D31" s="147" t="s">
+      <c r="D31" s="115" t="s">
         <v>42</v>
       </c>
       <c r="E31" s="205"/>
       <c r="F31" s="205"/>
       <c r="G31" s="206"/>
-      <c r="H31" s="150">
+      <c r="H31" s="116">
         <v>0</v>
       </c>
       <c r="I31" s="194"/>
       <c r="J31" s="63"/>
-      <c r="K31" s="155">
+      <c r="K31" s="118">
         <f t="shared" si="4"/>
         <v>17180</v>
       </c>
-      <c r="L31" s="156"/>
+      <c r="L31" s="119"/>
       <c r="M31" s="82">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -2916,22 +2918,22 @@
       <c r="A32" s="64"/>
       <c r="B32" s="69"/>
       <c r="C32" s="70"/>
-      <c r="D32" s="147" t="s">
+      <c r="D32" s="115" t="s">
         <v>43</v>
       </c>
       <c r="E32" s="205"/>
       <c r="F32" s="205"/>
       <c r="G32" s="206"/>
-      <c r="H32" s="150">
+      <c r="H32" s="116">
         <v>0</v>
       </c>
       <c r="I32" s="194"/>
       <c r="J32" s="63"/>
-      <c r="K32" s="155">
+      <c r="K32" s="118">
         <f t="shared" si="4"/>
         <v>4680</v>
       </c>
-      <c r="L32" s="156"/>
+      <c r="L32" s="119"/>
       <c r="M32" s="82">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -2945,22 +2947,22 @@
       <c r="A33" s="64"/>
       <c r="B33" s="69"/>
       <c r="C33" s="70"/>
-      <c r="D33" s="147" t="s">
+      <c r="D33" s="115" t="s">
         <v>44</v>
       </c>
       <c r="E33" s="205"/>
       <c r="F33" s="205"/>
       <c r="G33" s="206"/>
-      <c r="H33" s="150">
+      <c r="H33" s="116">
         <v>0</v>
       </c>
       <c r="I33" s="194"/>
       <c r="J33" s="63"/>
-      <c r="K33" s="155">
+      <c r="K33" s="118">
         <f t="shared" si="4"/>
         <v>4180</v>
       </c>
-      <c r="L33" s="156"/>
+      <c r="L33" s="119"/>
       <c r="M33" s="82">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -2974,22 +2976,22 @@
       <c r="A34" s="64"/>
       <c r="B34" s="69"/>
       <c r="C34" s="70"/>
-      <c r="D34" s="147" t="s">
+      <c r="D34" s="115" t="s">
         <v>45</v>
       </c>
       <c r="E34" s="205"/>
       <c r="F34" s="205"/>
       <c r="G34" s="206"/>
-      <c r="H34" s="150">
+      <c r="H34" s="116">
         <v>0</v>
       </c>
       <c r="I34" s="194"/>
       <c r="J34" s="63"/>
-      <c r="K34" s="155">
+      <c r="K34" s="118">
         <f t="shared" si="4"/>
         <v>9180</v>
       </c>
-      <c r="L34" s="156"/>
+      <c r="L34" s="119"/>
       <c r="M34" s="82">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -3003,22 +3005,22 @@
       <c r="A35" s="64"/>
       <c r="B35" s="69"/>
       <c r="C35" s="70"/>
-      <c r="D35" s="147" t="s">
+      <c r="D35" s="115" t="s">
         <v>46</v>
       </c>
       <c r="E35" s="205"/>
       <c r="F35" s="205"/>
       <c r="G35" s="206"/>
-      <c r="H35" s="150">
+      <c r="H35" s="116">
         <v>0</v>
       </c>
       <c r="I35" s="194"/>
       <c r="J35" s="63"/>
-      <c r="K35" s="155">
+      <c r="K35" s="118">
         <f t="shared" si="4"/>
         <v>11180</v>
       </c>
-      <c r="L35" s="156"/>
+      <c r="L35" s="119"/>
       <c r="M35" s="82">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -3032,22 +3034,22 @@
       <c r="A36" s="64"/>
       <c r="B36" s="69"/>
       <c r="C36" s="70"/>
-      <c r="D36" s="147" t="s">
+      <c r="D36" s="115" t="s">
         <v>47</v>
       </c>
       <c r="E36" s="205"/>
       <c r="F36" s="205"/>
       <c r="G36" s="206"/>
-      <c r="H36" s="150">
+      <c r="H36" s="116">
         <v>0</v>
       </c>
       <c r="I36" s="194"/>
       <c r="J36" s="63"/>
-      <c r="K36" s="155">
+      <c r="K36" s="118">
         <f t="shared" si="4"/>
         <v>10180</v>
       </c>
-      <c r="L36" s="156"/>
+      <c r="L36" s="119"/>
       <c r="M36" s="82">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -3061,22 +3063,22 @@
       <c r="A37" s="64"/>
       <c r="B37" s="69"/>
       <c r="C37" s="70"/>
-      <c r="D37" s="147" t="s">
+      <c r="D37" s="115" t="s">
         <v>48</v>
       </c>
       <c r="E37" s="205"/>
       <c r="F37" s="205"/>
       <c r="G37" s="206"/>
-      <c r="H37" s="150">
+      <c r="H37" s="116">
         <v>0</v>
       </c>
       <c r="I37" s="194"/>
       <c r="J37" s="63"/>
-      <c r="K37" s="155">
+      <c r="K37" s="118">
         <f t="shared" si="4"/>
         <v>5380</v>
       </c>
-      <c r="L37" s="156"/>
+      <c r="L37" s="119"/>
       <c r="M37" s="82">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -3090,22 +3092,22 @@
       <c r="A38" s="64"/>
       <c r="B38" s="69"/>
       <c r="C38" s="70"/>
-      <c r="D38" s="147" t="s">
+      <c r="D38" s="115" t="s">
         <v>49</v>
       </c>
       <c r="E38" s="205"/>
       <c r="F38" s="205"/>
       <c r="G38" s="206"/>
-      <c r="H38" s="150">
+      <c r="H38" s="116">
         <v>0</v>
       </c>
       <c r="I38" s="194"/>
       <c r="J38" s="63"/>
-      <c r="K38" s="155">
+      <c r="K38" s="118">
         <f t="shared" si="4"/>
-        <v>3960</v>
-      </c>
-      <c r="L38" s="156"/>
+        <v>3860</v>
+      </c>
+      <c r="L38" s="119"/>
       <c r="M38" s="82">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -3119,22 +3121,22 @@
       <c r="A39" s="64"/>
       <c r="B39" s="69"/>
       <c r="C39" s="70"/>
-      <c r="D39" s="147" t="s">
+      <c r="D39" s="115" t="s">
         <v>50</v>
       </c>
       <c r="E39" s="205"/>
       <c r="F39" s="205"/>
       <c r="G39" s="206"/>
-      <c r="H39" s="150">
+      <c r="H39" s="116">
         <v>0</v>
       </c>
       <c r="I39" s="194"/>
       <c r="J39" s="63"/>
-      <c r="K39" s="155">
+      <c r="K39" s="118">
         <f t="shared" si="4"/>
         <v>13680</v>
       </c>
-      <c r="L39" s="156"/>
+      <c r="L39" s="119"/>
       <c r="M39" s="82">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -3148,22 +3150,22 @@
       <c r="A40" s="64"/>
       <c r="B40" s="69"/>
       <c r="C40" s="70"/>
-      <c r="D40" s="147" t="s">
+      <c r="D40" s="115" t="s">
         <v>51</v>
       </c>
       <c r="E40" s="205"/>
       <c r="F40" s="205"/>
       <c r="G40" s="206"/>
-      <c r="H40" s="150">
+      <c r="H40" s="116">
         <v>0</v>
       </c>
       <c r="I40" s="194"/>
       <c r="J40" s="63"/>
-      <c r="K40" s="155">
+      <c r="K40" s="118">
         <f t="shared" si="4"/>
         <v>13680</v>
       </c>
-      <c r="L40" s="156"/>
+      <c r="L40" s="119"/>
       <c r="M40" s="82">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -3177,22 +3179,22 @@
       <c r="A41" s="64"/>
       <c r="B41" s="69"/>
       <c r="C41" s="70"/>
-      <c r="D41" s="147" t="s">
+      <c r="D41" s="115" t="s">
         <v>52</v>
       </c>
       <c r="E41" s="205"/>
       <c r="F41" s="205"/>
       <c r="G41" s="206"/>
-      <c r="H41" s="150">
+      <c r="H41" s="116">
         <v>0</v>
       </c>
       <c r="I41" s="194"/>
       <c r="J41" s="63"/>
-      <c r="K41" s="155">
+      <c r="K41" s="118">
         <f t="shared" si="4"/>
         <v>13680</v>
       </c>
-      <c r="L41" s="156"/>
+      <c r="L41" s="119"/>
       <c r="M41" s="82">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -3206,22 +3208,22 @@
       <c r="A42" s="64"/>
       <c r="B42" s="69"/>
       <c r="C42" s="70"/>
-      <c r="D42" s="147" t="s">
+      <c r="D42" s="115" t="s">
         <v>53</v>
       </c>
       <c r="E42" s="205"/>
       <c r="F42" s="205"/>
       <c r="G42" s="206"/>
-      <c r="H42" s="150">
+      <c r="H42" s="116">
         <v>0</v>
       </c>
       <c r="I42" s="194"/>
       <c r="J42" s="63"/>
-      <c r="K42" s="155">
+      <c r="K42" s="118">
         <f t="shared" si="4"/>
         <v>14680</v>
       </c>
-      <c r="L42" s="156"/>
+      <c r="L42" s="119"/>
       <c r="M42" s="82">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -3235,22 +3237,22 @@
       <c r="A43" s="64"/>
       <c r="B43" s="69"/>
       <c r="C43" s="70"/>
-      <c r="D43" s="147" t="s">
+      <c r="D43" s="115" t="s">
         <v>54</v>
       </c>
       <c r="E43" s="205"/>
       <c r="F43" s="205"/>
       <c r="G43" s="206"/>
-      <c r="H43" s="150">
+      <c r="H43" s="116">
         <v>0</v>
       </c>
       <c r="I43" s="194"/>
       <c r="J43" s="63"/>
-      <c r="K43" s="155">
+      <c r="K43" s="118">
         <f t="shared" si="4"/>
         <v>14680</v>
       </c>
-      <c r="L43" s="156"/>
+      <c r="L43" s="119"/>
       <c r="M43" s="82">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -3264,22 +3266,22 @@
       <c r="A44" s="64"/>
       <c r="B44" s="69"/>
       <c r="C44" s="70"/>
-      <c r="D44" s="147" t="s">
+      <c r="D44" s="115" t="s">
         <v>55</v>
       </c>
       <c r="E44" s="205"/>
       <c r="F44" s="205"/>
       <c r="G44" s="206"/>
-      <c r="H44" s="150">
+      <c r="H44" s="116">
         <v>0</v>
       </c>
       <c r="I44" s="194"/>
       <c r="J44" s="63"/>
-      <c r="K44" s="155">
+      <c r="K44" s="118">
         <f t="shared" si="4"/>
         <v>14680</v>
       </c>
-      <c r="L44" s="156"/>
+      <c r="L44" s="119"/>
       <c r="M44" s="82">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -3293,22 +3295,22 @@
       <c r="A45" s="64"/>
       <c r="B45" s="69"/>
       <c r="C45" s="70"/>
-      <c r="D45" s="147" t="s">
+      <c r="D45" s="115" t="s">
         <v>56</v>
       </c>
       <c r="E45" s="205"/>
       <c r="F45" s="205"/>
       <c r="G45" s="206"/>
-      <c r="H45" s="150">
+      <c r="H45" s="116">
         <v>0</v>
       </c>
       <c r="I45" s="194"/>
       <c r="J45" s="63"/>
-      <c r="K45" s="155">
+      <c r="K45" s="118">
         <f t="shared" si="4"/>
         <v>14680</v>
       </c>
-      <c r="L45" s="156"/>
+      <c r="L45" s="119"/>
       <c r="M45" s="82">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -3322,22 +3324,22 @@
       <c r="A46" s="64"/>
       <c r="B46" s="69"/>
       <c r="C46" s="70"/>
-      <c r="D46" s="147" t="s">
+      <c r="D46" s="115" t="s">
         <v>57</v>
       </c>
       <c r="E46" s="205"/>
       <c r="F46" s="205"/>
       <c r="G46" s="206"/>
-      <c r="H46" s="150">
+      <c r="H46" s="116">
         <v>0</v>
       </c>
       <c r="I46" s="194"/>
       <c r="J46" s="63"/>
-      <c r="K46" s="155">
+      <c r="K46" s="118">
         <f t="shared" si="4"/>
         <v>14680</v>
       </c>
-      <c r="L46" s="156"/>
+      <c r="L46" s="119"/>
       <c r="M46" s="82">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -3351,19 +3353,19 @@
       <c r="A47" s="64"/>
       <c r="B47" s="69"/>
       <c r="C47" s="70"/>
-      <c r="D47" s="149" t="s">
+      <c r="D47" s="127" t="s">
         <v>58</v>
       </c>
       <c r="E47" s="208"/>
       <c r="F47" s="208"/>
       <c r="G47" s="209"/>
-      <c r="H47" s="150">
+      <c r="H47" s="116">
         <v>0</v>
       </c>
       <c r="I47" s="194"/>
       <c r="J47" s="63"/>
-      <c r="K47" s="163"/>
-      <c r="L47" s="164"/>
+      <c r="K47" s="152"/>
+      <c r="L47" s="153"/>
       <c r="M47" s="79">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -3378,23 +3380,23 @@
     <row r="48" spans="1:17" ht="15.75" customHeight="1">
       <c r="A48" s="64"/>
       <c r="B48" s="69"/>
-      <c r="C48" s="145" t="s">
+      <c r="C48" s="131" t="s">
         <v>30</v>
       </c>
       <c r="D48" s="205"/>
       <c r="E48" s="205"/>
       <c r="F48" s="205"/>
       <c r="G48" s="206"/>
-      <c r="H48" s="150">
+      <c r="H48" s="116">
         <v>0</v>
       </c>
       <c r="I48" s="194"/>
       <c r="J48" s="63"/>
-      <c r="K48" s="155">
+      <c r="K48" s="118">
         <f>K38</f>
-        <v>3960</v>
-      </c>
-      <c r="L48" s="156"/>
+        <v>3860</v>
+      </c>
+      <c r="L48" s="119"/>
       <c r="M48" s="81">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -3410,23 +3412,23 @@
     <row r="49" spans="1:17" ht="15.75" customHeight="1">
       <c r="A49" s="64"/>
       <c r="B49" s="69"/>
-      <c r="C49" s="145" t="s">
+      <c r="C49" s="131" t="s">
         <v>31</v>
       </c>
       <c r="D49" s="205"/>
       <c r="E49" s="205"/>
       <c r="F49" s="205"/>
       <c r="G49" s="206"/>
-      <c r="H49" s="150">
+      <c r="H49" s="116">
         <v>0</v>
       </c>
       <c r="I49" s="194"/>
       <c r="J49" s="63"/>
-      <c r="K49" s="155">
+      <c r="K49" s="118">
         <f>K38</f>
-        <v>3960</v>
-      </c>
-      <c r="L49" s="156"/>
+        <v>3860</v>
+      </c>
+      <c r="L49" s="119"/>
       <c r="M49" s="81">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -3442,24 +3444,24 @@
     <row r="50" spans="1:17" ht="15.75" customHeight="1">
       <c r="A50" s="64"/>
       <c r="B50" s="69"/>
-      <c r="C50" s="145" t="s">
+      <c r="C50" s="131" t="s">
         <v>32</v>
       </c>
       <c r="D50" s="205"/>
       <c r="E50" s="205"/>
       <c r="F50" s="205"/>
       <c r="G50" s="206"/>
-      <c r="H50" s="146">
+      <c r="H50" s="136">
         <f>SUM(H51:I53)</f>
         <v>0</v>
       </c>
       <c r="I50" s="204"/>
       <c r="J50" s="63"/>
-      <c r="K50" s="155">
+      <c r="K50" s="118">
         <f>K38</f>
-        <v>3960</v>
-      </c>
-      <c r="L50" s="156"/>
+        <v>3860</v>
+      </c>
+      <c r="L50" s="119"/>
       <c r="M50" s="81">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -3476,19 +3478,19 @@
       <c r="A51" s="64"/>
       <c r="B51" s="69"/>
       <c r="C51" s="71"/>
-      <c r="D51" s="175" t="s">
+      <c r="D51" s="120" t="s">
         <v>33</v>
       </c>
-      <c r="E51" s="175"/>
-      <c r="F51" s="175"/>
-      <c r="G51" s="176"/>
-      <c r="H51" s="159">
-        <v>0</v>
-      </c>
-      <c r="I51" s="160"/>
+      <c r="E51" s="120"/>
+      <c r="F51" s="120"/>
+      <c r="G51" s="121"/>
+      <c r="H51" s="148">
+        <v>0</v>
+      </c>
+      <c r="I51" s="149"/>
       <c r="J51" s="74"/>
-      <c r="K51" s="161"/>
-      <c r="L51" s="162"/>
+      <c r="K51" s="150"/>
+      <c r="L51" s="151"/>
       <c r="M51" s="81"/>
       <c r="N51" s="95"/>
       <c r="O51" s="85"/>
@@ -3499,19 +3501,19 @@
       <c r="A52" s="64"/>
       <c r="B52" s="69"/>
       <c r="C52" s="70"/>
-      <c r="D52" s="147" t="s">
+      <c r="D52" s="115" t="s">
         <v>34</v>
       </c>
       <c r="E52" s="205"/>
       <c r="F52" s="205"/>
       <c r="G52" s="206"/>
-      <c r="H52" s="173">
+      <c r="H52" s="128">
         <v>0</v>
       </c>
       <c r="I52" s="194"/>
       <c r="J52" s="63"/>
-      <c r="K52" s="158"/>
-      <c r="L52" s="136"/>
+      <c r="K52" s="129"/>
+      <c r="L52" s="130"/>
       <c r="M52" s="81">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -3531,19 +3533,19 @@
       <c r="A53" s="64"/>
       <c r="B53" s="69"/>
       <c r="C53" s="70"/>
-      <c r="D53" s="149" t="s">
+      <c r="D53" s="127" t="s">
         <v>35</v>
       </c>
       <c r="E53" s="208"/>
       <c r="F53" s="208"/>
       <c r="G53" s="209"/>
-      <c r="H53" s="173">
+      <c r="H53" s="128">
         <v>0</v>
       </c>
       <c r="I53" s="194"/>
       <c r="J53" s="63"/>
-      <c r="K53" s="158"/>
-      <c r="L53" s="136"/>
+      <c r="K53" s="129"/>
+      <c r="L53" s="130"/>
       <c r="M53" s="81">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -3562,24 +3564,24 @@
     <row r="54" spans="1:17" ht="15.75" customHeight="1">
       <c r="A54" s="64"/>
       <c r="B54" s="69"/>
-      <c r="C54" s="145" t="s">
+      <c r="C54" s="131" t="s">
         <v>36</v>
       </c>
       <c r="D54" s="205"/>
       <c r="E54" s="205"/>
       <c r="F54" s="205"/>
       <c r="G54" s="206"/>
-      <c r="H54" s="146">
+      <c r="H54" s="136">
         <f>SUM(H55:I56)</f>
         <v>0</v>
       </c>
       <c r="I54" s="204"/>
       <c r="J54" s="63"/>
-      <c r="K54" s="155">
+      <c r="K54" s="118">
         <f>K38</f>
-        <v>3960</v>
-      </c>
-      <c r="L54" s="156"/>
+        <v>3860</v>
+      </c>
+      <c r="L54" s="119"/>
       <c r="M54" s="81">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -3596,18 +3598,18 @@
       <c r="A55" s="64"/>
       <c r="B55" s="69"/>
       <c r="C55" s="70"/>
-      <c r="D55" s="147" t="s">
+      <c r="D55" s="115" t="s">
         <v>37</v>
       </c>
       <c r="E55" s="205"/>
       <c r="F55" s="205"/>
       <c r="G55" s="206"/>
-      <c r="H55" s="173">
+      <c r="H55" s="128">
         <v>0</v>
       </c>
       <c r="I55" s="194"/>
       <c r="J55" s="63"/>
-      <c r="K55" s="173"/>
+      <c r="K55" s="128"/>
       <c r="L55" s="194"/>
       <c r="M55" s="81">
         <f t="shared" si="5"/>
@@ -3628,18 +3630,18 @@
       <c r="A56" s="64"/>
       <c r="B56" s="69"/>
       <c r="C56" s="70"/>
-      <c r="D56" s="147" t="s">
+      <c r="D56" s="115" t="s">
         <v>38</v>
       </c>
       <c r="E56" s="205"/>
       <c r="F56" s="205"/>
       <c r="G56" s="206"/>
-      <c r="H56" s="173">
+      <c r="H56" s="128">
         <v>0</v>
       </c>
       <c r="I56" s="194"/>
       <c r="J56" s="63"/>
-      <c r="K56" s="173"/>
+      <c r="K56" s="128"/>
       <c r="L56" s="194"/>
       <c r="M56" s="81">
         <f t="shared" si="5"/>
@@ -3658,7 +3660,7 @@
     </row>
     <row r="57" spans="1:17" ht="15.75" customHeight="1">
       <c r="A57" s="64"/>
-      <c r="B57" s="143" t="s">
+      <c r="B57" s="132" t="s">
         <v>59</v>
       </c>
       <c r="C57" s="202"/>
@@ -3669,7 +3671,7 @@
       <c r="H57" s="137"/>
       <c r="I57" s="192"/>
       <c r="J57" s="63"/>
-      <c r="K57" s="173"/>
+      <c r="K57" s="128"/>
       <c r="L57" s="194"/>
       <c r="M57" s="81">
         <f>SUM(M58:M59)</f>
@@ -3686,23 +3688,23 @@
     <row r="58" spans="1:17" ht="15.75" customHeight="1">
       <c r="A58" s="64"/>
       <c r="B58" s="105"/>
-      <c r="C58" s="145" t="s">
+      <c r="C58" s="131" t="s">
         <v>30</v>
       </c>
       <c r="D58" s="205"/>
       <c r="E58" s="205"/>
       <c r="F58" s="205"/>
       <c r="G58" s="206"/>
-      <c r="H58" s="148">
+      <c r="H58" s="133">
         <f>H48</f>
         <v>0</v>
       </c>
       <c r="I58" s="207"/>
       <c r="J58" s="63"/>
-      <c r="K58" s="182">
+      <c r="K58" s="123">
         <v>30000</v>
       </c>
-      <c r="L58" s="183"/>
+      <c r="L58" s="124"/>
       <c r="M58" s="82">
         <f t="shared" ref="M58:M62" si="9">H58*K58</f>
         <v>0</v>
@@ -3715,23 +3717,23 @@
     <row r="59" spans="1:17" ht="15.75" customHeight="1">
       <c r="A59" s="64"/>
       <c r="B59" s="105"/>
-      <c r="C59" s="145" t="s">
+      <c r="C59" s="131" t="s">
         <v>31</v>
       </c>
       <c r="D59" s="205"/>
       <c r="E59" s="205"/>
       <c r="F59" s="205"/>
       <c r="G59" s="206"/>
-      <c r="H59" s="148">
+      <c r="H59" s="133">
         <f>H49</f>
         <v>0</v>
       </c>
       <c r="I59" s="207"/>
       <c r="J59" s="63"/>
-      <c r="K59" s="182">
+      <c r="K59" s="123">
         <v>30000</v>
       </c>
-      <c r="L59" s="183"/>
+      <c r="L59" s="124"/>
       <c r="M59" s="82">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -3743,7 +3745,7 @@
     </row>
     <row r="60" spans="1:17" ht="15.75" customHeight="1">
       <c r="A60" s="64"/>
-      <c r="B60" s="143" t="s">
+      <c r="B60" s="132" t="s">
         <v>60</v>
       </c>
       <c r="C60" s="202"/>
@@ -3751,18 +3753,18 @@
       <c r="E60" s="202"/>
       <c r="F60" s="202"/>
       <c r="G60" s="203"/>
-      <c r="H60" s="148">
+      <c r="H60" s="133">
         <f>H16</f>
         <v>0</v>
       </c>
       <c r="I60" s="207"/>
-      <c r="J60" s="186">
-        <v>0</v>
-      </c>
-      <c r="K60" s="184">
-        <v>0</v>
-      </c>
-      <c r="L60" s="185"/>
+      <c r="J60" s="114">
+        <v>0</v>
+      </c>
+      <c r="K60" s="138">
+        <v>0</v>
+      </c>
+      <c r="L60" s="139"/>
       <c r="M60" s="81">
         <f>H60*J60*K60</f>
         <v>0</v>
@@ -3777,7 +3779,7 @@
     </row>
     <row r="61" spans="1:17" ht="15.75" customHeight="1">
       <c r="A61" s="64"/>
-      <c r="B61" s="143" t="s">
+      <c r="B61" s="132" t="s">
         <v>61</v>
       </c>
       <c r="C61" s="202"/>
@@ -3785,16 +3787,16 @@
       <c r="E61" s="202"/>
       <c r="F61" s="202"/>
       <c r="G61" s="203"/>
-      <c r="H61" s="148">
+      <c r="H61" s="133">
         <f>H16</f>
         <v>0</v>
       </c>
       <c r="I61" s="207"/>
       <c r="J61" s="63"/>
-      <c r="K61" s="182">
+      <c r="K61" s="123">
         <v>100</v>
       </c>
-      <c r="L61" s="183"/>
+      <c r="L61" s="124"/>
       <c r="M61" s="81">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -3809,7 +3811,7 @@
     </row>
     <row r="62" spans="1:17" ht="15.75" customHeight="1" thickBot="1">
       <c r="A62" s="106"/>
-      <c r="B62" s="171" t="s">
+      <c r="B62" s="134" t="s">
         <v>62</v>
       </c>
       <c r="C62" s="210"/>
@@ -3817,16 +3819,16 @@
       <c r="E62" s="210"/>
       <c r="F62" s="210"/>
       <c r="G62" s="211"/>
-      <c r="H62" s="172">
+      <c r="H62" s="135">
         <v>1</v>
       </c>
       <c r="I62" s="212"/>
       <c r="J62" s="65"/>
-      <c r="K62" s="178">
+      <c r="K62" s="125">
         <f>IF(NUMPAX&gt;=91,5000,LOOKUP(NUMPAX,CONTINGENCY_MATRIX,ContingencyMatrix!C1:C10))</f>
         <v>500</v>
       </c>
-      <c r="L62" s="179"/>
+      <c r="L62" s="126"/>
       <c r="M62" s="83">
         <f t="shared" si="9"/>
         <v>500</v>
@@ -3864,11 +3866,11 @@
       <c r="C64" s="52"/>
       <c r="D64" s="52"/>
       <c r="E64" s="52"/>
-      <c r="F64" s="174" t="s">
+      <c r="F64" s="117" t="s">
         <v>63</v>
       </c>
       <c r="G64" s="213"/>
-      <c r="H64" s="177"/>
+      <c r="H64" s="122"/>
       <c r="I64" s="214"/>
       <c r="J64" s="214"/>
       <c r="K64" s="214"/>
@@ -3894,11 +3896,11 @@
       <c r="C65" s="52"/>
       <c r="D65" s="52"/>
       <c r="E65" s="52"/>
-      <c r="F65" s="167" t="s">
+      <c r="F65" s="142" t="s">
         <v>64</v>
       </c>
       <c r="G65" s="215"/>
-      <c r="H65" s="168"/>
+      <c r="H65" s="143"/>
       <c r="I65" s="216"/>
       <c r="J65" s="216"/>
       <c r="K65" s="216"/>
@@ -3907,7 +3909,7 @@
         <f>M16+M28+M48+M49+M50+M54+M57+M61+M62</f>
         <v>500</v>
       </c>
-      <c r="N65" s="169"/>
+      <c r="N65" s="144"/>
       <c r="O65" s="217"/>
       <c r="P65" s="92">
         <f>SUM(N64:P64)</f>
@@ -3935,7 +3937,7 @@
       <c r="Q66" s="2"/>
     </row>
     <row r="67" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A67" s="170" t="s">
+      <c r="A67" s="145" t="s">
         <v>65</v>
       </c>
       <c r="B67" s="218"/>
@@ -3982,45 +3984,45 @@
     </row>
     <row r="69" spans="1:17" ht="15.75" customHeight="1">
       <c r="A69" s="66"/>
-      <c r="B69" s="165"/>
-      <c r="C69" s="165"/>
-      <c r="D69" s="165"/>
-      <c r="E69" s="165"/>
-      <c r="F69" s="165"/>
+      <c r="B69" s="140"/>
+      <c r="C69" s="140"/>
+      <c r="D69" s="140"/>
+      <c r="E69" s="140"/>
+      <c r="F69" s="140"/>
       <c r="G69" s="66"/>
-      <c r="H69" s="165"/>
+      <c r="H69" s="140"/>
       <c r="I69" s="219"/>
       <c r="J69" s="219"/>
       <c r="K69" s="219"/>
       <c r="L69" s="219"/>
-      <c r="M69" s="166"/>
+      <c r="M69" s="141"/>
       <c r="N69" s="220"/>
-      <c r="O69" s="166"/>
+      <c r="O69" s="141"/>
       <c r="P69" s="220"/>
       <c r="Q69" s="2"/>
     </row>
     <row r="70" spans="1:17" ht="15.75" customHeight="1">
       <c r="A70" s="66"/>
-      <c r="B70" s="165" t="s">
+      <c r="B70" s="140" t="s">
         <v>69</v>
       </c>
-      <c r="C70" s="165"/>
-      <c r="D70" s="165"/>
-      <c r="E70" s="165"/>
-      <c r="F70" s="165"/>
+      <c r="C70" s="140"/>
+      <c r="D70" s="140"/>
+      <c r="E70" s="140"/>
+      <c r="F70" s="140"/>
       <c r="G70" s="66"/>
-      <c r="H70" s="165" t="s">
+      <c r="H70" s="140" t="s">
         <v>70</v>
       </c>
       <c r="I70" s="219"/>
       <c r="J70" s="219"/>
       <c r="K70" s="219"/>
       <c r="L70" s="219"/>
-      <c r="M70" s="166" t="s">
+      <c r="M70" s="141" t="s">
         <v>71</v>
       </c>
       <c r="N70" s="220"/>
-      <c r="O70" s="166" t="s">
+      <c r="O70" s="141" t="s">
         <v>72</v>
       </c>
       <c r="P70" s="220"/>
@@ -5056,8 +5058,169 @@
     <protectedRange sqref="F3" name="Range22"/>
     <protectedRange sqref="K17:L20" name="Range23"/>
     <protectedRange sqref="K24:L24" name="Range24"/>
+    <protectedRange sqref="F7" name="Range25"/>
+    <protectedRange sqref="F7:O7" name="Activity Title"/>
+    <protectedRange sqref="O13:P13" name="Venue"/>
   </protectedRanges>
   <mergeCells count="182">
+    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F3:O3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="F4:O4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="F5:O5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="F7:O7"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="F11:O11"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="A15:G15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="P3:P11"/>
+    <mergeCell ref="F10:O10"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="F9:O9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="L8:N8"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="D21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="D23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="D45:G45"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="D25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="D29:G29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="D33:G33"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="D34:G34"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="D35:G35"/>
+    <mergeCell ref="D41:G41"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="D42:G42"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="D43:G43"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="D44:G44"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="D31:G31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="K38:L38"/>
+    <mergeCell ref="D37:G37"/>
+    <mergeCell ref="D38:G38"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="D36:G36"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="K35:L35"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="K37:L37"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="D30:G30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="H51:I51"/>
+    <mergeCell ref="K51:L51"/>
+    <mergeCell ref="H59:I59"/>
+    <mergeCell ref="C59:G59"/>
+    <mergeCell ref="K46:L46"/>
+    <mergeCell ref="K47:L47"/>
+    <mergeCell ref="D46:G46"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="D47:G47"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="C48:G48"/>
+    <mergeCell ref="H48:I48"/>
+    <mergeCell ref="K48:L48"/>
+    <mergeCell ref="H49:I49"/>
+    <mergeCell ref="K49:L49"/>
+    <mergeCell ref="C49:G49"/>
+    <mergeCell ref="C50:G50"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="K50:L50"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="H70:L70"/>
+    <mergeCell ref="M70:N70"/>
+    <mergeCell ref="O70:P70"/>
+    <mergeCell ref="F65:G65"/>
+    <mergeCell ref="H65:L65"/>
+    <mergeCell ref="N65:O65"/>
+    <mergeCell ref="A67:D67"/>
+    <mergeCell ref="H69:L69"/>
+    <mergeCell ref="M69:N69"/>
+    <mergeCell ref="O69:P69"/>
+    <mergeCell ref="B69:F69"/>
+    <mergeCell ref="B70:F70"/>
+    <mergeCell ref="H61:I61"/>
+    <mergeCell ref="B62:G62"/>
+    <mergeCell ref="H62:I62"/>
+    <mergeCell ref="D52:G52"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="K52:L52"/>
+    <mergeCell ref="K54:L54"/>
+    <mergeCell ref="H54:I54"/>
+    <mergeCell ref="D55:G55"/>
+    <mergeCell ref="H55:I55"/>
+    <mergeCell ref="D56:G56"/>
+    <mergeCell ref="H56:I56"/>
+    <mergeCell ref="B57:G57"/>
+    <mergeCell ref="H57:I57"/>
+    <mergeCell ref="C58:G58"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="K55:L55"/>
+    <mergeCell ref="K56:L56"/>
+    <mergeCell ref="K57:L57"/>
+    <mergeCell ref="K58:L58"/>
+    <mergeCell ref="K59:L59"/>
+    <mergeCell ref="B60:G60"/>
+    <mergeCell ref="H60:I60"/>
+    <mergeCell ref="K60:L60"/>
     <mergeCell ref="D32:G32"/>
     <mergeCell ref="H32:I32"/>
     <mergeCell ref="F64:G64"/>
@@ -5082,164 +5245,6 @@
     <mergeCell ref="K53:L53"/>
     <mergeCell ref="C54:G54"/>
     <mergeCell ref="B61:G61"/>
-    <mergeCell ref="H61:I61"/>
-    <mergeCell ref="B62:G62"/>
-    <mergeCell ref="H62:I62"/>
-    <mergeCell ref="D52:G52"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="K52:L52"/>
-    <mergeCell ref="K54:L54"/>
-    <mergeCell ref="H54:I54"/>
-    <mergeCell ref="D55:G55"/>
-    <mergeCell ref="H55:I55"/>
-    <mergeCell ref="D56:G56"/>
-    <mergeCell ref="H56:I56"/>
-    <mergeCell ref="B57:G57"/>
-    <mergeCell ref="H57:I57"/>
-    <mergeCell ref="C58:G58"/>
-    <mergeCell ref="H58:I58"/>
-    <mergeCell ref="K55:L55"/>
-    <mergeCell ref="K56:L56"/>
-    <mergeCell ref="K57:L57"/>
-    <mergeCell ref="K58:L58"/>
-    <mergeCell ref="K59:L59"/>
-    <mergeCell ref="B60:G60"/>
-    <mergeCell ref="H60:I60"/>
-    <mergeCell ref="K60:L60"/>
-    <mergeCell ref="H70:L70"/>
-    <mergeCell ref="M70:N70"/>
-    <mergeCell ref="O70:P70"/>
-    <mergeCell ref="F65:G65"/>
-    <mergeCell ref="H65:L65"/>
-    <mergeCell ref="N65:O65"/>
-    <mergeCell ref="A67:D67"/>
-    <mergeCell ref="H69:L69"/>
-    <mergeCell ref="M69:N69"/>
-    <mergeCell ref="O69:P69"/>
-    <mergeCell ref="B69:F69"/>
-    <mergeCell ref="B70:F70"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="H51:I51"/>
-    <mergeCell ref="K51:L51"/>
-    <mergeCell ref="H59:I59"/>
-    <mergeCell ref="C59:G59"/>
-    <mergeCell ref="K46:L46"/>
-    <mergeCell ref="K47:L47"/>
-    <mergeCell ref="D46:G46"/>
-    <mergeCell ref="H46:I46"/>
-    <mergeCell ref="D47:G47"/>
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="C48:G48"/>
-    <mergeCell ref="H48:I48"/>
-    <mergeCell ref="K48:L48"/>
-    <mergeCell ref="H49:I49"/>
-    <mergeCell ref="K49:L49"/>
-    <mergeCell ref="C49:G49"/>
-    <mergeCell ref="C50:G50"/>
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="K50:L50"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="D44:G44"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="D31:G31"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="D22:G22"/>
-    <mergeCell ref="K38:L38"/>
-    <mergeCell ref="D37:G37"/>
-    <mergeCell ref="D38:G38"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="D36:G36"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="K35:L35"/>
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="K37:L37"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="D30:G30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="D45:G45"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="D25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="D29:G29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="D33:G33"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="D34:G34"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="D35:G35"/>
-    <mergeCell ref="D41:G41"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="D42:G42"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="D43:G43"/>
-    <mergeCell ref="H43:I43"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="D21:G21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="D23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="F11:O11"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="A15:G15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="P3:P11"/>
-    <mergeCell ref="F10:O10"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="F9:O9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="L8:N8"/>
-    <mergeCell ref="A1:Q1"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="F3:O3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="F4:O4"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="F5:O5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="F7:O7"/>
   </mergeCells>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K61" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -5431,7 +5436,7 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:27" ht="15.6">
-      <c r="A3" s="180" t="s">
+      <c r="A3" s="185" t="s">
         <v>75</v>
       </c>
       <c r="B3" s="221"/>
@@ -5446,7 +5451,7 @@
       <c r="K3" s="221"/>
       <c r="L3" s="221"/>
       <c r="M3" s="222"/>
-      <c r="N3" s="181"/>
+      <c r="N3" s="186"/>
       <c r="O3" s="221"/>
       <c r="P3" s="221"/>
       <c r="Q3" s="221"/>
@@ -6731,7 +6736,7 @@
     </row>
     <row r="23" spans="1:23" ht="15.75" customHeight="1">
       <c r="A23" s="15" t="s">
-        <v>19</v>
+        <v>98</v>
       </c>
       <c r="B23" s="16">
         <v>2200</v>
@@ -6800,7 +6805,7 @@
     </row>
     <row r="24" spans="1:23" ht="15.75" customHeight="1">
       <c r="A24" s="15" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B24" s="16">
         <v>2200</v>
@@ -6869,7 +6874,7 @@
     </row>
     <row r="25" spans="1:23" ht="15.75" customHeight="1">
       <c r="A25" s="15" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B25" s="16">
         <v>1800</v>
@@ -6938,7 +6943,7 @@
     </row>
     <row r="26" spans="1:23" ht="15.75" customHeight="1">
       <c r="A26" s="15" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B26" s="16">
         <v>1800</v>
@@ -7076,7 +7081,7 @@
     </row>
     <row r="28" spans="1:23" ht="15.75" customHeight="1">
       <c r="A28" s="15" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B28" s="16">
         <v>1800</v>
@@ -7145,7 +7150,7 @@
     </row>
     <row r="29" spans="1:23" ht="15.75" customHeight="1">
       <c r="A29" s="15" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B29" s="16">
         <v>1500</v>
@@ -7283,7 +7288,7 @@
     </row>
     <row r="31" spans="1:23" ht="15.75" customHeight="1">
       <c r="A31" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B31" s="16">
         <v>1500</v>
@@ -7352,7 +7357,7 @@
     </row>
     <row r="32" spans="1:23" ht="15.75" customHeight="1">
       <c r="A32" s="15" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B32" s="16">
         <v>1500</v>
@@ -7421,7 +7426,7 @@
     </row>
     <row r="33" spans="1:23" ht="15.75" customHeight="1">
       <c r="A33" s="15" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B33" s="16">
         <v>1800</v>
@@ -7490,7 +7495,7 @@
     </row>
     <row r="34" spans="1:23" ht="15.75" customHeight="1">
       <c r="A34" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B34" s="16">
         <v>2200</v>
@@ -7559,7 +7564,7 @@
     </row>
     <row r="35" spans="1:23" ht="15.75" customHeight="1">
       <c r="A35" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B35" s="16">
         <v>1500</v>
@@ -7628,7 +7633,7 @@
     </row>
     <row r="36" spans="1:23" ht="15.75" customHeight="1">
       <c r="A36" s="15" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B36" s="16">
         <v>2200</v>
@@ -7697,7 +7702,7 @@
     </row>
     <row r="37" spans="1:23" ht="15.75" customHeight="1">
       <c r="A37" s="15" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B37" s="16">
         <v>1800</v>
@@ -7766,7 +7771,7 @@
     </row>
     <row r="38" spans="1:23" ht="15.75" customHeight="1">
       <c r="A38" s="15" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B38" s="16">
         <v>2200</v>
@@ -7835,7 +7840,7 @@
     </row>
     <row r="39" spans="1:23" ht="15.75" customHeight="1">
       <c r="A39" s="15" t="s">
-        <v>111</v>
+        <v>19</v>
       </c>
       <c r="B39" s="16">
         <v>2200</v>

</xml_diff>